<commit_message>
Adding Alsea perm in new form
</commit_message>
<xml_diff>
--- a/templates/perms/docs/Alsea-cues.xlsx
+++ b/templates/perms/docs/Alsea-cues.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="460" windowWidth="19980" windowHeight="17300" tabRatio="500"/>
+    <workbookView xWindow="12260" yWindow="460" windowWidth="15320" windowHeight="17300" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="cuesheet.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Cue sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Control distances" sheetId="2" r:id="rId2"/>
+    <sheet name="RWGPS" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">cuesheet.csv!$A$1:$H$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Cue sheet'!$A$1:$H$64</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="168">
   <si>
     <t>Control</t>
     <phoneticPr fontId="13" type="noConversion"/>
@@ -173,9 +175,6 @@
     <t>Snyder Rd</t>
   </si>
   <si>
-    <t>Continue Snyder Rd as it turns R then L</t>
-  </si>
-  <si>
     <t>Goodman Rd</t>
   </si>
   <si>
@@ -197,16 +196,10 @@
     <t>R/L (SS)</t>
   </si>
   <si>
-    <t>Fern Ridge Path (not toward Roosevelt)</t>
-  </si>
-  <si>
     <t>Terry St (watch for traffic)</t>
   </si>
   <si>
     <t>Fern Ridge Trail (back onto bike path)</t>
-  </si>
-  <si>
-    <t>Small bridge over canal, then larger bridge over 18th Street into park</t>
   </si>
   <si>
     <t>Miles</t>
@@ -275,21 +268,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>Left off path in school parking lot; follow path east through school grounds toward street</t>
-  </si>
-  <si>
-    <t>Polk St</t>
-  </si>
-  <si>
-    <t>W 24th Ave</t>
-  </si>
-  <si>
-    <t>R (SS)</t>
-  </si>
-  <si>
-    <t>Friendly St</t>
-  </si>
-  <si>
     <t>L (SL)</t>
   </si>
   <si>
@@ -306,9 +284,6 @@
 [Control open / Control close]</t>
   </si>
   <si>
-    <t>Bear left onto Lorane Hwy (no right turn)</t>
-  </si>
-  <si>
     <t>Continue 0.1 mile on OR-34 to Post Office</t>
   </si>
   <si>
@@ -316,9 +291,6 @@
   </si>
   <si>
     <t>OR-99W S  (coming into Monroe again; good refuel stop)</t>
-  </si>
-  <si>
-    <t>At Green Hill Road, right then left onto bike path</t>
   </si>
   <si>
     <t>Leg</t>
@@ -344,10 +316,6 @@
   </si>
   <si>
     <t>Option:  McFarland recommended only for tires 32mm or wider. Skinny tire riders may continue on Alpine, R on Bellfountain (blinking light); rejoin main route at Dawson and Bellfountain.  About 4 miles, 1 mile bonus.</t>
-  </si>
-  <si>
-    <t>Alsea Loop brevet from Eugene, OR 
-Permanent #1726 - modification pending RUSA approval</t>
   </si>
   <si>
     <t>Control: DS Market in Crow at Territorial Road and Central Road [Open +0:50, Close +1:40]</t>
@@ -370,7 +338,247 @@
     <t>Finish control at Market of Choice, 29th and Willamette (turn into lot before the intersection).  Additional food available at Pegasus Pizza, 16 Tons Pour House,  others   [Open +6:48, Close + 13:36]</t>
   </si>
   <si>
-    <t>Begin at 29th and Willamette, Eugene OR.  Market of Choice, 7-11. Exit shopping center right onto 29th Ave (up the hill, west) [Open +00:00, close +1:00 ]</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Distance (miles) From Start</t>
+  </si>
+  <si>
+    <t>Elevation (ft)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Start of route</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Slight right onto Lorane Hwy</t>
+  </si>
+  <si>
+    <t>Straight</t>
+  </si>
+  <si>
+    <t>Continue onto Spencer Creek Rd</t>
+  </si>
+  <si>
+    <t>Continue onto Pine Grove Rd</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Turn left to stay on Pine Grove Rd</t>
+  </si>
+  <si>
+    <t>Continue onto Erickson Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto Crow Rd</t>
+  </si>
+  <si>
+    <t>Turn right onto Territorial Rd</t>
+  </si>
+  <si>
+    <t>Slight right onto Applegate Trail</t>
+  </si>
+  <si>
+    <t>Turn left onto OR-36 W/State Hwy 36 W</t>
+  </si>
+  <si>
+    <t>Turn right onto Territorial Hwy</t>
+  </si>
+  <si>
+    <t>Turn left onto OR-99W N/Pacific Hwy W</t>
+  </si>
+  <si>
+    <t>Hors Category</t>
+  </si>
+  <si>
+    <t>Control: Monroe</t>
+  </si>
+  <si>
+    <t>Turn left onto Alpine Cut Off Rd</t>
+  </si>
+  <si>
+    <t>Turn right onto McFarland Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto Occidental Ln</t>
+  </si>
+  <si>
+    <t>Slight left onto Dawson Rd</t>
+  </si>
+  <si>
+    <t>Slight right onto Bellfountain Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto Decker Rd</t>
+  </si>
+  <si>
+    <t>Keep right to stay on Decker Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto OR-34 W</t>
+  </si>
+  <si>
+    <t>Control: Alsea</t>
+  </si>
+  <si>
+    <t>Turn right onto S 1st St/Alsea-Deadwood Hwy</t>
+  </si>
+  <si>
+    <t>Turn left onto S Fork Rd</t>
+  </si>
+  <si>
+    <t>Summit</t>
+  </si>
+  <si>
+    <t>Turn right onto OR-99W S</t>
+  </si>
+  <si>
+    <t>Turn right onto S 5th St/Territorial Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto Ferguson Rd</t>
+  </si>
+  <si>
+    <t>Information Control</t>
+  </si>
+  <si>
+    <t>Sharp right onto Washburn Ln</t>
+  </si>
+  <si>
+    <t>Turn left onto High Pass Rd</t>
+  </si>
+  <si>
+    <t>Turn right onto Dorsey Ln</t>
+  </si>
+  <si>
+    <t>Continue onto Alvadore Rd</t>
+  </si>
+  <si>
+    <t>Turn left to stay on Alvadore Rd</t>
+  </si>
+  <si>
+    <t>Turn left to stay on Snyder Rd</t>
+  </si>
+  <si>
+    <t>Turn right onto Goodman Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto Clear Lake Rd</t>
+  </si>
+  <si>
+    <t>Turn right onto Fir Butte Rd</t>
+  </si>
+  <si>
+    <t>Slight left to stay on Fir Butte Rd</t>
+  </si>
+  <si>
+    <t>Continue onto Bodenhamer Rd</t>
+  </si>
+  <si>
+    <t>Slight right onto Fir Butte Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto Royal Ave</t>
+  </si>
+  <si>
+    <t>Turn right onto Green Hill Rd</t>
+  </si>
+  <si>
+    <t>Turn left onto Fern Ridge Path</t>
+  </si>
+  <si>
+    <t>Turn right to stay on Fern Ridge Path</t>
+  </si>
+  <si>
+    <t>Turn left onto Terry St</t>
+  </si>
+  <si>
+    <t>Turn right onto Fern Ridge Trail</t>
+  </si>
+  <si>
+    <t>Turn left to stay on Fern Ridge Trail</t>
+  </si>
+  <si>
+    <t>Slight left to stay on Fern Ridge Trail</t>
+  </si>
+  <si>
+    <t>Turn left onto City View St</t>
+  </si>
+  <si>
+    <t>Turn right onto Polk St</t>
+  </si>
+  <si>
+    <t>Continue onto W 29th Ave</t>
+  </si>
+  <si>
+    <t>Turn left toward W 29th Ave</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>End of route</t>
+  </si>
+  <si>
+    <t>Slight left onto Lorane Hwy</t>
+  </si>
+  <si>
+    <t>Turn right onto Friendly St</t>
+  </si>
+  <si>
+    <t>Continue onto W 16th Ave</t>
+  </si>
+  <si>
+    <t>Turn left toward W 16th Ave</t>
+  </si>
+  <si>
+    <t>Keep right to stay on Fern Ridge Trail</t>
+  </si>
+  <si>
+    <t>Onto 16th Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R </t>
+  </si>
+  <si>
+    <t>Friendly St (do not reenter path)</t>
+  </si>
+  <si>
+    <t>Begin at 29th and Willamette, Eugene OR.  Market of Choice, 7-11. Exit shopping center right onto 29th Ave (up the hill, west; becomes Lorane Hwy) [Open +00:00, close +1:00 ]</t>
+  </si>
+  <si>
+    <t>Bear left at traffic island to continue Lorane Hwy</t>
+  </si>
+  <si>
+    <t>Alpine Rd</t>
+  </si>
+  <si>
+    <t>At Green Hill Road, right then left onto Fern Ridge bike path</t>
+  </si>
+  <si>
+    <t>To stay on Fern Ridge Path (not toward Roosevelt)</t>
+  </si>
+  <si>
+    <t>dog leg left City View, then right to continue Fern Ridge Trail</t>
+  </si>
+  <si>
+    <t>Underpass; stay on Fern Ridge trail</t>
+  </si>
+  <si>
+    <t>Jog right onto Polk, across canal, left to continue Fern Ridge Trail (now on south side of canal)</t>
   </si>
 </sst>
 </file>
@@ -382,7 +590,7 @@
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -463,6 +671,18 @@
       <i/>
       <sz val="16"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -579,10 +799,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -700,6 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -710,7 +935,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1045,17 +1274,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="6" style="10" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="58.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="3.33203125" style="3" hidden="1" customWidth="1"/>
@@ -1065,62 +1293,60 @@
     <col min="10" max="10" width="6.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="39"/>
+    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="40"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
-        <v>92</v>
-      </c>
+      <c r="D1" s="16"/>
       <c r="E1" s="17"/>
       <c r="F1" s="15"/>
-      <c r="G1" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="39"/>
+      <c r="G1" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="40"/>
       <c r="I1" s="8"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A3" s="21"/>
       <c r="B3" s="22">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="23" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="E3" s="24">
         <f t="shared" ref="E3:E33" si="0">1.60934*B3</f>
@@ -1135,49 +1361,49 @@
     <row r="4" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="28">
         <f t="shared" ref="A4:A10" si="1">B4-B3</f>
-        <v>0.21</v>
+        <v>0.3</v>
       </c>
       <c r="B4" s="22">
-        <v>0.21</v>
+        <v>0.3</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="E4" s="24">
         <f t="shared" si="0"/>
-        <v>0.33796139999999997</v>
+        <v>0.48280199999999995</v>
       </c>
       <c r="F4" s="30">
         <f t="shared" ref="F4:F33" si="2">E4-E3</f>
-        <v>0.33796139999999997</v>
+        <v>0.48280199999999995</v>
       </c>
       <c r="G4" s="31">
         <f>A4/0.625</f>
-        <v>0.33599999999999997</v>
+        <v>0.48</v>
       </c>
       <c r="H4" s="32">
         <f>B4*1.609344</f>
-        <v>0.33796224000000002</v>
+        <v>0.48280319999999999</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J10" si="3">$J$64*(E4/15)</f>
-        <v>9.3878166666667398E-4</v>
+        <f>$J$63*(E4/15)</f>
+        <v>1.341116666666677E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="28">
         <f t="shared" si="1"/>
-        <v>5.5200000000000005</v>
+        <v>5.4300000000000006</v>
       </c>
       <c r="B5" s="22">
         <v>5.73</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>10</v>
@@ -1188,19 +1414,19 @@
       </c>
       <c r="F5" s="30">
         <f t="shared" si="2"/>
-        <v>8.8835568000000009</v>
+        <v>8.7387162000000007</v>
       </c>
       <c r="G5" s="31">
-        <f t="shared" ref="G5:G63" si="4">A5/0.625</f>
-        <v>8.8320000000000007</v>
+        <f t="shared" ref="G5:G62" si="3">A5/0.625</f>
+        <v>8.6880000000000006</v>
       </c>
       <c r="H5" s="32">
-        <f t="shared" ref="H5:H63" si="5">B5*1.609344</f>
+        <f t="shared" ref="H5:H62" si="4">B5*1.609344</f>
         <v>9.2215411200000013</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="1">
-        <f t="shared" si="3"/>
+        <f>$J$63*(E5/15)</f>
         <v>2.5615328333333538E-2</v>
       </c>
     </row>
@@ -1227,16 +1453,16 @@
         <v>5.2786352000000001</v>
       </c>
       <c r="G6" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.2479999999999993</v>
       </c>
       <c r="H6" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>14.50018944</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="1">
-        <f t="shared" si="3"/>
+        <f>$J$63*(E6/15)</f>
         <v>4.0278203888889211E-2</v>
       </c>
     </row>
@@ -1263,16 +1489,16 @@
         <v>1.1104445999999992</v>
       </c>
       <c r="G7" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.1039999999999992</v>
       </c>
       <c r="H7" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>15.6106368</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="1">
-        <f t="shared" si="3"/>
+        <f>$J$63*(E7/15)</f>
         <v>4.3362772222222568E-2</v>
       </c>
     </row>
@@ -1299,16 +1525,16 @@
         <v>2.6554110000000009</v>
       </c>
       <c r="G8" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2.6400000000000006</v>
       </c>
       <c r="H8" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>18.266054400000002</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="1">
-        <f t="shared" si="3"/>
+        <f>$J$63*(E8/15)</f>
         <v>5.0738913888889299E-2</v>
       </c>
     </row>
@@ -1335,16 +1561,16 @@
         <v>5.2947285999999991</v>
       </c>
       <c r="G9" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.2640000000000011</v>
       </c>
       <c r="H9" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>23.560796160000002</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="1">
-        <f t="shared" si="3"/>
+        <f>$J$63*(E9/15)</f>
         <v>6.5446493333333841E-2</v>
       </c>
     </row>
@@ -1360,7 +1586,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E10" s="24">
         <f t="shared" si="0"/>
@@ -1371,16 +1597,16 @@
         <v>1.5449663999999999</v>
       </c>
       <c r="G10" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.5359999999999985</v>
       </c>
       <c r="H10" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>25.1057664</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="1">
-        <f t="shared" si="3"/>
+        <f>$J$63*(E10/15)</f>
         <v>6.9738066666667223E-2</v>
       </c>
     </row>
@@ -1389,16 +1615,16 @@
       <c r="B11" s="22"/>
       <c r="C11" s="21"/>
       <c r="D11" s="23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="30"/>
       <c r="G11" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H11" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I11" s="13"/>
@@ -1427,22 +1653,22 @@
         <v>20.036283000000001</v>
       </c>
       <c r="G12" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21.456</v>
       </c>
       <c r="H12" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>45.142099200000004</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="1">
-        <f t="shared" ref="J12:J27" si="6">$J$64*(E12/15)</f>
+        <f>$J$63*(E12/15)</f>
         <v>0.12539440833333435</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="28">
-        <f t="shared" ref="A13:A19" si="7">B13-B12</f>
+        <f t="shared" ref="A13:A19" si="5">B13-B12</f>
         <v>2.6099999999999994</v>
       </c>
       <c r="B13" s="22">
@@ -1463,22 +1689,22 @@
         <v>4.2003774000000007</v>
       </c>
       <c r="G13" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.1759999999999993</v>
       </c>
       <c r="H13" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>49.342487040000002</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E13/15)</f>
         <v>0.13706212333333442</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.26999999999999957</v>
       </c>
       <c r="B14" s="22">
@@ -1499,22 +1725,22 @@
         <v>0.43452179999999885</v>
       </c>
       <c r="G14" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.43199999999999933</v>
       </c>
       <c r="H14" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>49.777009920000005</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E14/15)</f>
         <v>0.13826912833333443</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8.6700000000000017</v>
       </c>
       <c r="B15" s="22">
@@ -1535,22 +1761,22 @@
         <v>13.952977799999999</v>
       </c>
       <c r="G15" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13.872000000000003</v>
       </c>
       <c r="H15" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63.73002240000001</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E15/15)</f>
         <v>0.17702740000000139</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A16" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="B16" s="22">
@@ -1560,7 +1786,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E16" s="24">
         <f t="shared" si="0"/>
@@ -1571,22 +1797,22 @@
         <v>0</v>
       </c>
       <c r="G16" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H16" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>63.73002240000001</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E16/15)</f>
         <v>0.17702740000000139</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="B17" s="22">
@@ -1596,7 +1822,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E17" s="24">
         <f t="shared" si="0"/>
@@ -1607,32 +1833,32 @@
         <v>1.609339999999996</v>
       </c>
       <c r="G17" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
       <c r="H17" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>65.339366400000003</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E17/15)</f>
         <v>0.18149778888889032</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.85999999999999943</v>
       </c>
       <c r="B18" s="22">
         <v>41.46</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>25</v>
+        <v>162</v>
       </c>
       <c r="E18" s="24">
         <f t="shared" si="0"/>
@@ -1643,22 +1869,22 @@
         <v>1.3840324000000095</v>
       </c>
       <c r="G18" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.375999999999999</v>
       </c>
       <c r="H18" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>66.723402240000013</v>
       </c>
       <c r="I18" s="13"/>
       <c r="J18" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E18/15)</f>
         <v>0.18534232333333481</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.85000000000000142</v>
       </c>
       <c r="B19" s="22">
@@ -1668,7 +1894,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" si="0"/>
@@ -1679,16 +1905,16 @@
         <v>1.3679389999999927</v>
       </c>
       <c r="G19" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.3600000000000023</v>
       </c>
       <c r="H19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>68.091344640000003</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E19/15)</f>
         <v>0.18914215388889039</v>
       </c>
     </row>
@@ -1697,16 +1923,16 @@
       <c r="B20" s="22"/>
       <c r="C20" s="21"/>
       <c r="D20" s="29" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="30"/>
       <c r="G20" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H20" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I20" s="13"/>
@@ -1724,7 +1950,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E21" s="24">
         <f t="shared" si="0"/>
@@ -1735,22 +1961,22 @@
         <v>3.1703997999999984</v>
       </c>
       <c r="G21" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.1519999999999984</v>
       </c>
       <c r="H21" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>71.261752320000014</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E21/15)</f>
         <v>0.19794882000000155</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="28">
-        <f t="shared" ref="A22:A27" si="8">B22-B21</f>
+        <f t="shared" ref="A22:A27" si="6">B22-B21</f>
         <v>0.61999999999999744</v>
       </c>
       <c r="B22" s="22">
@@ -1771,22 +1997,22 @@
         <v>0.9977908000000042</v>
       </c>
       <c r="G22" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.99199999999999589</v>
       </c>
       <c r="H22" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>72.259545599999996</v>
       </c>
       <c r="I22" s="13"/>
       <c r="J22" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E22/15)</f>
         <v>0.20072046111111272</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.64999999999999858</v>
       </c>
       <c r="B23" s="22">
@@ -1807,22 +2033,22 @@
         <v>1.0460709999999978</v>
       </c>
       <c r="G23" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0399999999999978</v>
       </c>
       <c r="H23" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>73.305619199999995</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E23/15)</f>
         <v>0.20362621388889049</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>7.5600000000000023</v>
       </c>
       <c r="B24" s="22">
@@ -1841,22 +2067,22 @@
         <v>12.166610399999996</v>
       </c>
       <c r="G24" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>12.096000000000004</v>
       </c>
       <c r="H24" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>85.472259840000007</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E24/15)</f>
         <v>0.23742235388889077</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B25" s="22">
@@ -1877,22 +2103,22 @@
         <v>0</v>
       </c>
       <c r="G25" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H25" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>85.472259840000007</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E25/15)</f>
         <v>0.23742235388889077</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>7.1400000000000006</v>
       </c>
       <c r="B26" s="22">
@@ -1913,22 +2139,22 @@
         <v>11.490687600000001</v>
       </c>
       <c r="G26" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>11.424000000000001</v>
       </c>
       <c r="H26" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>96.962976000000012</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E26/15)</f>
         <v>0.26934093055555769</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A27" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>11.950000000000003</v>
       </c>
       <c r="B27" s="22">
@@ -1936,7 +2162,7 @@
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="23" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E27" s="24">
         <f t="shared" si="0"/>
@@ -1947,16 +2173,16 @@
         <v>19.23161300000001</v>
       </c>
       <c r="G27" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19.120000000000005</v>
       </c>
       <c r="H27" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>116.19463680000001</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="1">
-        <f t="shared" si="6"/>
+        <f>$J$63*(E27/15)</f>
         <v>0.32276207777778038</v>
       </c>
     </row>
@@ -1965,16 +2191,16 @@
       <c r="B28" s="22"/>
       <c r="C28" s="21"/>
       <c r="D28" s="23" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="30"/>
       <c r="G28" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H28" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I28" s="13"/>
@@ -2003,16 +2229,16 @@
         <v>9.6560400000001323E-2</v>
       </c>
       <c r="G29" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9.6000000000003638E-2</v>
       </c>
       <c r="H29" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>116.29119744000002</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="1">
-        <f>$J$64*(E29/15)</f>
+        <f>$J$63*(E29/15)</f>
         <v>0.32303030111111369</v>
       </c>
     </row>
@@ -2039,26 +2265,26 @@
         <v>1.5449663999999927</v>
       </c>
       <c r="G30" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.53599999999999</v>
       </c>
       <c r="H30" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>117.83616768</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="1">
-        <f>$J$64*(E30/15)</f>
+        <f>$J$63*(E30/15)</f>
         <v>0.32732187444444705</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="28">
         <f>B31-B30</f>
-        <v>12.420000000000002</v>
+        <v>12.879999999999995</v>
       </c>
       <c r="B31" s="22">
-        <v>85.64</v>
+        <v>86.1</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>19</v>
@@ -2068,33 +2294,33 @@
       </c>
       <c r="E31" s="24">
         <f t="shared" si="0"/>
-        <v>137.8238776</v>
+        <v>138.56417399999998</v>
       </c>
       <c r="F31" s="30">
         <f t="shared" si="2"/>
-        <v>19.988002800000004</v>
+        <v>20.728299199999981</v>
       </c>
       <c r="G31" s="31">
-        <f t="shared" si="4"/>
-        <v>19.872000000000003</v>
+        <f t="shared" si="3"/>
+        <v>20.607999999999993</v>
       </c>
       <c r="H31" s="32">
-        <f t="shared" si="5"/>
-        <v>137.82422016000001</v>
+        <f t="shared" si="4"/>
+        <v>138.5645184</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="1">
-        <f>$J$64*(E31/15)</f>
-        <v>0.3828441044444475</v>
+        <f>$J$63*(E31/15)</f>
+        <v>0.38490048333333637</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="28">
         <f>B32-B31</f>
-        <v>8.019999999999996</v>
+        <v>8.0200000000000102</v>
       </c>
       <c r="B32" s="22">
-        <v>93.66</v>
+        <v>94.12</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>11</v>
@@ -2104,24 +2330,24 @@
       </c>
       <c r="E32" s="24">
         <f t="shared" si="0"/>
-        <v>150.7307844</v>
+        <v>151.47108080000001</v>
       </c>
       <c r="F32" s="30">
         <f t="shared" si="2"/>
-        <v>12.906906800000002</v>
+        <v>12.90690680000003</v>
       </c>
       <c r="G32" s="31">
-        <f t="shared" si="4"/>
-        <v>12.831999999999994</v>
+        <f t="shared" si="3"/>
+        <v>12.832000000000017</v>
       </c>
       <c r="H32" s="32">
-        <f t="shared" si="5"/>
-        <v>150.73115903999999</v>
+        <f t="shared" si="4"/>
+        <v>151.47145728000001</v>
       </c>
       <c r="I32" s="13"/>
       <c r="J32" s="1">
-        <f>$J$64*(E32/15)</f>
-        <v>0.41869662333333668</v>
+        <f>$J$63*(E32/15)</f>
+        <v>0.42075300222222561</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="14" x14ac:dyDescent="0.15">
@@ -2130,43 +2356,43 @@
         <v>0.85999999999999943</v>
       </c>
       <c r="B33" s="22">
-        <v>94.52</v>
+        <v>94.98</v>
       </c>
       <c r="C33" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E33" s="24">
         <f t="shared" si="0"/>
-        <v>152.1148168</v>
+        <v>152.85511320000001</v>
       </c>
       <c r="F33" s="30">
         <f t="shared" si="2"/>
         <v>1.3840323999999953</v>
       </c>
       <c r="G33" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.375999999999999</v>
       </c>
       <c r="H33" s="32">
-        <f t="shared" si="5"/>
-        <v>152.11519487999999</v>
+        <f t="shared" si="4"/>
+        <v>152.85549312000001</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="1">
-        <f>$J$64*(E33/15)</f>
-        <v>0.42254115777778112</v>
+        <f>$J$63*(E33/15)</f>
+        <v>0.42459753666667005</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="28">
         <f>B34-B33</f>
-        <v>0.98000000000000398</v>
+        <v>0.96999999999999886</v>
       </c>
       <c r="B34" s="22">
-        <v>95.5</v>
+        <v>95.95</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>11</v>
@@ -2177,65 +2403,65 @@
       <c r="E34" s="24"/>
       <c r="F34" s="30"/>
       <c r="G34" s="31">
-        <f t="shared" si="4"/>
-        <v>1.5680000000000063</v>
+        <f t="shared" si="3"/>
+        <v>1.5519999999999983</v>
       </c>
       <c r="H34" s="32">
-        <f t="shared" si="5"/>
-        <v>153.692352</v>
+        <f t="shared" si="4"/>
+        <v>154.41655680000002</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="28">
-        <f t="shared" ref="A35:A36" si="9">B35-B34</f>
-        <v>4.9000000000000057</v>
+        <f t="shared" ref="A35:A36" si="7">B35-B34</f>
+        <v>4.4299999999999926</v>
       </c>
       <c r="B35" s="22">
-        <v>100.4</v>
+        <v>100.38</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="30"/>
       <c r="G35" s="31">
-        <f t="shared" si="4"/>
-        <v>7.8400000000000087</v>
+        <f t="shared" si="3"/>
+        <v>7.0879999999999885</v>
       </c>
       <c r="H35" s="32">
-        <f t="shared" si="5"/>
-        <v>161.57813760000002</v>
+        <f t="shared" si="4"/>
+        <v>161.54595072000001</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="28">
-        <f t="shared" si="9"/>
-        <v>2.0999999999999943</v>
+        <f t="shared" si="7"/>
+        <v>2.1200000000000045</v>
       </c>
       <c r="B36" s="22">
         <v>102.5</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="30"/>
       <c r="G36" s="31">
-        <f t="shared" si="4"/>
-        <v>3.359999999999991</v>
+        <f t="shared" si="3"/>
+        <v>3.3920000000000075</v>
       </c>
       <c r="H36" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164.95776000000001</v>
       </c>
       <c r="I36" s="13"/>
@@ -2248,16 +2474,16 @@
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="30"/>
       <c r="G37" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H37" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>164.95776000000001</v>
       </c>
       <c r="I37" s="13"/>
@@ -2266,10 +2492,10 @@
     <row r="38" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="28">
         <f>B38-B36</f>
-        <v>1.7999999999999972</v>
+        <v>2.5499999999999972</v>
       </c>
       <c r="B38" s="22">
-        <v>104.3</v>
+        <v>105.05</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>23</v>
@@ -2278,34 +2504,34 @@
         <v>36</v>
       </c>
       <c r="E38" s="24">
-        <f t="shared" ref="E38:E63" si="10">1.60934*B38</f>
-        <v>167.854162</v>
+        <f t="shared" ref="E38:E62" si="8">1.60934*B38</f>
+        <v>169.06116699999998</v>
       </c>
       <c r="F38" s="30" t="e">
         <f>E38-#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="G38" s="31">
-        <f t="shared" si="4"/>
-        <v>2.8799999999999955</v>
+        <f t="shared" si="3"/>
+        <v>4.0799999999999956</v>
       </c>
       <c r="H38" s="32">
-        <f t="shared" si="5"/>
-        <v>167.85457920000002</v>
+        <f t="shared" si="4"/>
+        <v>169.06158720000002</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="1">
-        <f t="shared" ref="J38:J63" si="11">$J$64*(E38/15)</f>
-        <v>0.46626156111111478</v>
+        <f>$J$63*(E38/15)</f>
+        <v>0.46961435277778141</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="28">
         <f>B39-B38</f>
-        <v>1.2999999999999972</v>
+        <v>0.5</v>
       </c>
       <c r="B39" s="22">
-        <v>105.6</v>
+        <v>105.55</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>11</v>
@@ -2314,34 +2540,34 @@
         <v>37</v>
       </c>
       <c r="E39" s="24">
-        <f t="shared" si="10"/>
-        <v>169.946304</v>
+        <f t="shared" si="8"/>
+        <v>169.865837</v>
       </c>
       <c r="F39" s="30">
-        <f t="shared" ref="F39:F63" si="12">E39-E38</f>
-        <v>2.0921419999999955</v>
+        <f t="shared" ref="F39:F62" si="9">E39-E38</f>
+        <v>0.80467000000001576</v>
       </c>
       <c r="G39" s="31">
-        <f t="shared" si="4"/>
-        <v>2.0799999999999956</v>
+        <f t="shared" si="3"/>
+        <v>0.8</v>
       </c>
       <c r="H39" s="32">
-        <f t="shared" si="5"/>
-        <v>169.94672639999999</v>
+        <f t="shared" si="4"/>
+        <v>169.8662592</v>
       </c>
       <c r="I39" s="13"/>
       <c r="J39" s="1">
-        <f t="shared" si="11"/>
-        <v>0.47207306666667043</v>
+        <f>$J$63*(E39/15)</f>
+        <v>0.471849547222226</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="28">
         <f>B40-B39</f>
-        <v>1.5</v>
+        <v>1.5400000000000063</v>
       </c>
       <c r="B40" s="22">
-        <v>107.1</v>
+        <v>107.09</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>19</v>
@@ -2350,60 +2576,60 @@
         <v>38</v>
       </c>
       <c r="E40" s="24">
-        <f t="shared" si="10"/>
-        <v>172.36031399999999</v>
+        <f t="shared" si="8"/>
+        <v>172.3442206</v>
       </c>
       <c r="F40" s="30">
-        <f t="shared" si="12"/>
-        <v>2.4140099999999904</v>
+        <f t="shared" si="9"/>
+        <v>2.4783836000000008</v>
       </c>
       <c r="G40" s="31">
-        <f t="shared" si="4"/>
-        <v>2.4</v>
+        <f t="shared" si="3"/>
+        <v>2.4640000000000102</v>
       </c>
       <c r="H40" s="32">
-        <f t="shared" si="5"/>
-        <v>172.36074239999999</v>
+        <f t="shared" si="4"/>
+        <v>172.34464896000003</v>
       </c>
       <c r="I40" s="13"/>
       <c r="J40" s="1">
-        <f t="shared" si="11"/>
-        <v>0.47877865000000375</v>
+        <f>$J$63*(E40/15)</f>
+        <v>0.47873394611111486</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="28">
         <f>B41-B40</f>
-        <v>1.9000000000000057</v>
+        <v>1.9099999999999966</v>
       </c>
       <c r="B41" s="22">
         <v>109</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="D41" s="29" t="s">
         <v>39</v>
       </c>
       <c r="E41" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>175.41806</v>
       </c>
       <c r="F41" s="30">
-        <f t="shared" si="12"/>
-        <v>3.0577460000000087</v>
+        <f t="shared" si="9"/>
+        <v>3.0738393999999971</v>
       </c>
       <c r="G41" s="31">
-        <f t="shared" si="4"/>
-        <v>3.0400000000000089</v>
+        <f t="shared" si="3"/>
+        <v>3.0559999999999947</v>
       </c>
       <c r="H41" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>175.418496</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="1">
-        <f t="shared" si="11"/>
+        <f>$J$63*(E41/15)</f>
         <v>0.48727238888889274</v>
       </c>
     </row>
@@ -2422,7 +2648,7 @@
         <v>41</v>
       </c>
       <c r="E42" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>180.728882</v>
       </c>
       <c r="F42" s="30" t="e">
@@ -2430,16 +2656,16 @@
         <v>#REF!</v>
       </c>
       <c r="G42" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.2799999999999958</v>
       </c>
       <c r="H42" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>180.72933120000002</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="1">
-        <f t="shared" si="11"/>
+        <f>$J$63*(E42/15)</f>
         <v>0.50202467222222624</v>
       </c>
     </row>
@@ -2458,776 +2684,740 @@
         <v>42</v>
       </c>
       <c r="E43" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>182.338222</v>
       </c>
       <c r="F43" s="30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>1.6093400000000031</v>
       </c>
       <c r="G43" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
       <c r="H43" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>182.33867520000001</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="1">
-        <f t="shared" si="11"/>
+        <f>$J$63*(E43/15)</f>
         <v>0.5064950611111152</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="42" x14ac:dyDescent="0.15">
-      <c r="A44" s="28"/>
+      <c r="A44" s="28">
+        <f>B44-B43</f>
+        <v>0</v>
+      </c>
       <c r="B44" s="22">
         <v>113.3</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="23" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E44" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>182.338222</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H44" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>182.33867520000001</v>
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="7">
-        <f t="shared" si="11"/>
+        <f>$J$63*(E44/15)</f>
         <v>0.5064950611111152</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="28">
-        <f>B45-B43</f>
-        <v>0.5</v>
+        <f>B45-B44</f>
+        <v>0.93999999999999773</v>
       </c>
       <c r="B45" s="22">
-        <v>113.8</v>
+        <v>114.24</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D45" s="29" t="s">
         <v>43</v>
       </c>
       <c r="E45" s="24">
-        <f t="shared" si="10"/>
-        <v>183.14289199999999</v>
-      </c>
-      <c r="F45" s="30">
-        <f>E45-E43</f>
-        <v>0.80466999999998734</v>
+        <f t="shared" si="8"/>
+        <v>183.85100159999999</v>
+      </c>
+      <c r="F45" s="30" t="e">
+        <f>E45-#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="G45" s="31">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
+        <f t="shared" si="3"/>
+        <v>1.5039999999999965</v>
       </c>
       <c r="H45" s="32">
-        <f t="shared" si="5"/>
-        <v>183.14334719999999</v>
+        <f t="shared" si="4"/>
+        <v>183.85145856</v>
       </c>
       <c r="I45" s="13"/>
       <c r="J45" s="1">
-        <f t="shared" si="11"/>
-        <v>0.50873025555555951</v>
+        <f>$J$63*(E45/15)</f>
+        <v>0.51069722666667072</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="28">
-        <f t="shared" ref="A46:A63" si="13">B46-B45</f>
-        <v>0.5</v>
+        <f t="shared" ref="A46:A62" si="10">B46-B45</f>
+        <v>0.37000000000000455</v>
       </c>
       <c r="B46" s="22">
-        <v>114.3</v>
+        <v>114.61</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D46" s="29" t="s">
         <v>44</v>
       </c>
       <c r="E46" s="24">
-        <f t="shared" si="10"/>
-        <v>183.947562</v>
+        <f t="shared" si="8"/>
+        <v>184.44645739999999</v>
       </c>
       <c r="F46" s="30">
-        <f>E46-E45</f>
-        <v>0.80467000000001576</v>
+        <f t="shared" si="9"/>
+        <v>0.59545579999999632</v>
       </c>
       <c r="G46" s="31">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
+        <f t="shared" si="3"/>
+        <v>0.5920000000000073</v>
       </c>
       <c r="H46" s="32">
-        <f t="shared" si="5"/>
-        <v>183.9480192</v>
+        <f t="shared" si="4"/>
+        <v>184.44691584</v>
       </c>
       <c r="I46" s="13"/>
       <c r="J46" s="1">
-        <f t="shared" si="11"/>
-        <v>0.51096545000000415</v>
+        <f>$J$63*(E46/15)</f>
+        <v>0.51235127055555962</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="28">
-        <f t="shared" si="13"/>
-        <v>0.29999999999999716</v>
+        <f t="shared" si="10"/>
+        <v>0.48999999999999488</v>
       </c>
       <c r="B47" s="22">
-        <v>114.6</v>
+        <v>115.1</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D47" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E47" s="24">
-        <f t="shared" si="10"/>
-        <v>184.430364</v>
+        <f t="shared" si="8"/>
+        <v>185.23503399999998</v>
       </c>
       <c r="F47" s="30">
-        <f t="shared" si="12"/>
-        <v>0.4828019999999924</v>
+        <f t="shared" si="9"/>
+        <v>0.78857659999999896</v>
       </c>
       <c r="G47" s="31">
-        <f t="shared" si="4"/>
-        <v>0.47999999999999543</v>
+        <f t="shared" si="3"/>
+        <v>0.78399999999999181</v>
       </c>
       <c r="H47" s="32">
-        <f t="shared" si="5"/>
-        <v>184.43082240000001</v>
+        <f t="shared" si="4"/>
+        <v>185.23549439999999</v>
       </c>
       <c r="I47" s="13"/>
       <c r="J47" s="1">
-        <f t="shared" si="11"/>
-        <v>0.51230656666667074</v>
+        <f>$J$63*(E47/15)</f>
+        <v>0.51454176111111516</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="28">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f t="shared" si="10"/>
+        <v>1.0300000000000011</v>
       </c>
       <c r="B48" s="22">
-        <v>115.1</v>
+        <v>116.13</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E48" s="24">
-        <f t="shared" si="10"/>
-        <v>185.23503399999998</v>
+        <f t="shared" si="8"/>
+        <v>186.89265419999998</v>
       </c>
       <c r="F48" s="30">
-        <f t="shared" si="12"/>
-        <v>0.80466999999998734</v>
+        <f t="shared" si="9"/>
+        <v>1.6576201999999967</v>
       </c>
       <c r="G48" s="31">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
+        <f t="shared" si="3"/>
+        <v>1.6480000000000019</v>
       </c>
       <c r="H48" s="32">
-        <f t="shared" si="5"/>
-        <v>185.23549439999999</v>
+        <f t="shared" si="4"/>
+        <v>186.89311872000002</v>
       </c>
       <c r="I48" s="13"/>
       <c r="J48" s="1">
-        <f t="shared" si="11"/>
-        <v>0.51454176111111516</v>
+        <f>$J$63*(E48/15)</f>
+        <v>0.51914626166667066</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="28">
-        <f t="shared" si="13"/>
-        <v>1.1000000000000085</v>
+        <f t="shared" si="10"/>
+        <v>1.6800000000000068</v>
       </c>
       <c r="B49" s="22">
-        <v>116.2</v>
+        <v>117.81</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D49" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E49" s="24">
-        <f t="shared" si="10"/>
-        <v>187.00530800000001</v>
+        <f t="shared" si="8"/>
+        <v>189.59634539999999</v>
       </c>
       <c r="F49" s="30">
-        <f t="shared" si="12"/>
-        <v>1.770274000000029</v>
+        <f t="shared" si="9"/>
+        <v>2.7036912000000086</v>
       </c>
       <c r="G49" s="31">
-        <f t="shared" si="4"/>
-        <v>1.7600000000000136</v>
+        <f t="shared" si="3"/>
+        <v>2.6880000000000108</v>
       </c>
       <c r="H49" s="32">
-        <f t="shared" si="5"/>
-        <v>187.00577280000002</v>
+        <f t="shared" si="4"/>
+        <v>189.59681664000001</v>
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="1">
-        <f t="shared" si="11"/>
-        <v>0.51945918888889309</v>
+        <f>$J$63*(E49/15)</f>
+        <v>0.52665651500000421</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="28">
-        <f t="shared" si="13"/>
-        <v>1.7000000000000028</v>
+        <f t="shared" si="10"/>
+        <v>1.3100000000000023</v>
       </c>
       <c r="B50" s="22">
-        <v>117.9</v>
+        <v>119.12</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="E50" s="24">
-        <f t="shared" si="10"/>
-        <v>189.741186</v>
+        <f t="shared" si="8"/>
+        <v>191.7045808</v>
       </c>
       <c r="F50" s="30">
-        <f t="shared" si="12"/>
-        <v>2.7358779999999854</v>
+        <f t="shared" si="9"/>
+        <v>2.1082354000000123</v>
       </c>
       <c r="G50" s="31">
-        <f t="shared" si="4"/>
-        <v>2.7200000000000046</v>
+        <f t="shared" si="3"/>
+        <v>2.0960000000000036</v>
       </c>
       <c r="H50" s="32">
-        <f t="shared" si="5"/>
-        <v>189.74165760000002</v>
+        <f t="shared" si="4"/>
+        <v>191.70505728000003</v>
       </c>
       <c r="I50" s="13"/>
       <c r="J50" s="1">
-        <f t="shared" si="11"/>
-        <v>0.52705885000000419</v>
+        <f>$J$63*(E50/15)</f>
+        <v>0.53251272444444864</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="28">
-        <f t="shared" si="13"/>
-        <v>1.2999999999999972</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="B51" s="22">
-        <v>119.2</v>
+        <v>120.12</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
       <c r="E51" s="24">
-        <f t="shared" si="10"/>
-        <v>191.83332799999999</v>
+        <f t="shared" si="8"/>
+        <v>193.31392080000001</v>
       </c>
       <c r="F51" s="30">
-        <f t="shared" si="12"/>
-        <v>2.0921419999999955</v>
+        <f t="shared" si="9"/>
+        <v>1.6093400000000031</v>
       </c>
       <c r="G51" s="31">
-        <f t="shared" si="4"/>
-        <v>2.0799999999999956</v>
+        <f t="shared" si="3"/>
+        <v>1.6</v>
       </c>
       <c r="H51" s="32">
-        <f t="shared" si="5"/>
-        <v>191.83380480000002</v>
+        <f t="shared" si="4"/>
+        <v>193.31440128000003</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="1">
-        <f t="shared" si="11"/>
-        <v>0.53287035555555973</v>
+        <f>$J$63*(E51/15)</f>
+        <v>0.53698311333333759</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="28">
-        <f t="shared" si="13"/>
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>0.94999999999998863</v>
       </c>
       <c r="B52" s="22">
-        <v>120.2</v>
+        <v>121.07</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" s="24">
-        <f t="shared" si="10"/>
-        <v>193.442668</v>
+        <f t="shared" si="8"/>
+        <v>194.84279379999998</v>
       </c>
       <c r="F52" s="30">
-        <f t="shared" si="12"/>
-        <v>1.6093400000000031</v>
+        <f t="shared" si="9"/>
+        <v>1.5288729999999759</v>
       </c>
       <c r="G52" s="31">
-        <f t="shared" si="4"/>
-        <v>1.6</v>
+        <f t="shared" si="3"/>
+        <v>1.5199999999999818</v>
       </c>
       <c r="H52" s="32">
-        <f t="shared" si="5"/>
-        <v>193.44314880000002</v>
+        <f t="shared" si="4"/>
+        <v>194.84327808</v>
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="1">
-        <f t="shared" si="11"/>
-        <v>0.53734074444444868</v>
+        <f>$J$63*(E52/15)</f>
+        <v>0.541229982777782</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="28">
-        <f t="shared" si="13"/>
-        <v>0.89999999999999147</v>
+        <f t="shared" si="10"/>
+        <v>4.0000000000006253E-2</v>
       </c>
       <c r="B53" s="22">
-        <v>121.1</v>
+        <v>121.11</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53" s="24">
-        <f t="shared" si="10"/>
-        <v>194.891074</v>
+        <f t="shared" si="8"/>
+        <v>194.90716739999999</v>
       </c>
       <c r="F53" s="30">
-        <f t="shared" si="12"/>
-        <v>1.4484060000000056</v>
+        <f t="shared" si="9"/>
+        <v>6.4373600000010356E-2</v>
       </c>
       <c r="G53" s="31">
-        <f t="shared" si="4"/>
-        <v>1.4399999999999864</v>
+        <f t="shared" si="3"/>
+        <v>6.4000000000010007E-2</v>
       </c>
       <c r="H53" s="32">
-        <f t="shared" si="5"/>
-        <v>194.89155840000001</v>
+        <f t="shared" si="4"/>
+        <v>194.90765184</v>
       </c>
       <c r="I53" s="13"/>
       <c r="J53" s="1">
-        <f t="shared" si="11"/>
-        <v>0.54136409444444877</v>
+        <f>$J$63*(E53/15)</f>
+        <v>0.54140879833333766</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="28">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.1899999999999977</v>
       </c>
       <c r="B54" s="22">
-        <v>121.1</v>
+        <v>124.3</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>53</v>
+        <v>165</v>
       </c>
       <c r="E54" s="24">
+        <f t="shared" si="8"/>
+        <v>200.04096200000001</v>
+      </c>
+      <c r="F54" s="30"/>
+      <c r="G54" s="31">
+        <f t="shared" si="3"/>
+        <v>5.1039999999999965</v>
+      </c>
+      <c r="H54" s="32">
+        <f t="shared" si="4"/>
+        <v>200.04145920000002</v>
+      </c>
+      <c r="I54" s="13"/>
+      <c r="J54" s="7">
+        <f>$J$63*(E54/15)</f>
+        <v>0.55566933888889336</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="A55" s="28">
         <f t="shared" si="10"/>
-        <v>194.891074</v>
-      </c>
-      <c r="F54" s="30">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G54" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="32">
-        <f t="shared" si="5"/>
-        <v>194.89155840000001</v>
-      </c>
-      <c r="I54" s="13"/>
-      <c r="J54" s="1">
-        <f t="shared" si="11"/>
-        <v>0.54136409444444877</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="28" x14ac:dyDescent="0.15">
-      <c r="A55" s="28">
-        <f t="shared" si="13"/>
-        <v>4</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="B55" s="22">
-        <v>125.1</v>
+        <v>124.9</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="E55" s="24">
-        <f t="shared" si="10"/>
-        <v>201.32843399999999</v>
-      </c>
-      <c r="F55" s="30">
-        <f t="shared" si="12"/>
-        <v>6.437359999999984</v>
-      </c>
+        <f t="shared" si="8"/>
+        <v>201.00656600000002</v>
+      </c>
+      <c r="F55" s="30"/>
       <c r="G55" s="31">
-        <f t="shared" si="4"/>
-        <v>6.4</v>
+        <f t="shared" si="3"/>
+        <v>0.96000000000001362</v>
       </c>
       <c r="H55" s="32">
-        <f t="shared" si="5"/>
-        <v>201.32893440000001</v>
+        <f t="shared" si="4"/>
+        <v>201.00706560000003</v>
       </c>
       <c r="I55" s="13"/>
-      <c r="J55" s="1">
-        <f t="shared" si="11"/>
-        <v>0.55924565000000437</v>
+      <c r="J55" s="7">
+        <f>$J$63*(E55/15)</f>
+        <v>0.55835157222222676</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A56" s="28">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f>B56-B53</f>
+        <v>4.1200000000000045</v>
       </c>
       <c r="B56" s="22">
-        <v>125.6</v>
+        <v>125.23</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="E56" s="24">
-        <f t="shared" si="10"/>
-        <v>202.133104</v>
+        <f t="shared" si="8"/>
+        <v>201.53764820000001</v>
       </c>
       <c r="F56" s="30">
-        <f t="shared" si="12"/>
-        <v>0.80467000000001576</v>
+        <f>E56-E53</f>
+        <v>6.6304808000000151</v>
       </c>
       <c r="G56" s="31">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
+        <f t="shared" si="3"/>
+        <v>6.5920000000000076</v>
       </c>
       <c r="H56" s="32">
-        <f t="shared" si="5"/>
-        <v>202.13360639999999</v>
+        <f t="shared" si="4"/>
+        <v>201.53814912000001</v>
       </c>
       <c r="I56" s="13"/>
       <c r="J56" s="1">
-        <f t="shared" si="11"/>
-        <v>0.5614808444444489</v>
+        <f>$J$63*(E56/15)</f>
+        <v>0.55982680055556</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="28">
-        <f t="shared" si="13"/>
-        <v>0.20000000000000284</v>
+        <f t="shared" si="10"/>
+        <v>0.17000000000000171</v>
       </c>
       <c r="B57" s="22">
-        <v>125.8</v>
+        <v>125.4</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>70</v>
+        <v>157</v>
       </c>
       <c r="E57" s="24">
-        <f t="shared" si="10"/>
-        <v>202.454972</v>
+        <f t="shared" si="8"/>
+        <v>201.81123600000001</v>
       </c>
       <c r="F57" s="30">
-        <f t="shared" si="12"/>
-        <v>0.32186799999999494</v>
+        <f t="shared" si="9"/>
+        <v>0.27358780000000138</v>
       </c>
       <c r="G57" s="31">
-        <f t="shared" si="4"/>
-        <v>0.32000000000000456</v>
+        <f t="shared" si="3"/>
+        <v>0.27200000000000274</v>
       </c>
       <c r="H57" s="32">
-        <f t="shared" si="5"/>
-        <v>202.4554752</v>
+        <f t="shared" si="4"/>
+        <v>201.81173760000001</v>
       </c>
       <c r="I57" s="13"/>
       <c r="J57" s="1">
-        <f t="shared" si="11"/>
-        <v>0.56237492222222674</v>
+        <f>$J$63*(E57/15)</f>
+        <v>0.56058676666667118</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="28">
-        <f t="shared" si="13"/>
-        <v>0.10000000000000853</v>
+        <f t="shared" si="10"/>
+        <v>0.19999999999998863</v>
       </c>
       <c r="B58" s="22">
-        <v>125.9</v>
+        <v>125.6</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="E58" s="24">
-        <f t="shared" si="10"/>
-        <v>202.615906</v>
-      </c>
-      <c r="F58" s="30">
-        <f t="shared" si="12"/>
-        <v>0.16093399999999747</v>
+        <f t="shared" si="8"/>
+        <v>202.133104</v>
+      </c>
+      <c r="F58" s="30" t="e">
+        <f>E58-#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="G58" s="31">
-        <f t="shared" si="4"/>
-        <v>0.16000000000001363</v>
+        <f t="shared" si="3"/>
+        <v>0.3199999999999818</v>
       </c>
       <c r="H58" s="32">
-        <f t="shared" si="5"/>
-        <v>202.61640960000003</v>
+        <f t="shared" si="4"/>
+        <v>202.13360639999999</v>
       </c>
       <c r="I58" s="13"/>
       <c r="J58" s="1">
-        <f t="shared" si="11"/>
-        <v>0.5628219611111156</v>
+        <f>$J$63*(E58/15)</f>
+        <v>0.5614808444444489</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="28">
-        <f t="shared" si="13"/>
-        <v>0.39999999999999147</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="B59" s="22">
-        <v>126.3</v>
+        <v>126.6</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E59" s="24">
-        <f t="shared" si="10"/>
-        <v>203.25964199999999</v>
+        <f t="shared" si="8"/>
+        <v>203.74244399999998</v>
       </c>
       <c r="F59" s="30">
-        <f t="shared" si="12"/>
-        <v>0.64373599999998987</v>
+        <f t="shared" si="9"/>
+        <v>1.6093399999999747</v>
       </c>
       <c r="G59" s="31">
-        <f t="shared" si="4"/>
-        <v>0.63999999999998636</v>
+        <f t="shared" si="3"/>
+        <v>1.6</v>
       </c>
       <c r="H59" s="32">
-        <f t="shared" si="5"/>
-        <v>203.26014720000001</v>
+        <f t="shared" si="4"/>
+        <v>203.74295040000001</v>
       </c>
       <c r="I59" s="13"/>
       <c r="J59" s="1">
-        <f t="shared" si="11"/>
-        <v>0.56461011666667105</v>
+        <f>$J$63*(E59/15)</f>
+        <v>0.56595123333333774</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="28">
-        <f t="shared" si="13"/>
-        <v>0.29999999999999716</v>
+        <f t="shared" si="10"/>
+        <v>0.30000000000001137</v>
       </c>
       <c r="B60" s="22">
-        <v>126.6</v>
+        <v>126.9</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E60" s="24">
-        <f t="shared" si="10"/>
-        <v>203.74244399999998</v>
+        <f t="shared" si="8"/>
+        <v>204.225246</v>
       </c>
       <c r="F60" s="30">
-        <f t="shared" si="12"/>
-        <v>0.4828019999999924</v>
+        <f t="shared" si="9"/>
+        <v>0.48280200000002083</v>
       </c>
       <c r="G60" s="31">
-        <f t="shared" si="4"/>
-        <v>0.47999999999999543</v>
+        <f t="shared" si="3"/>
+        <v>0.48000000000001819</v>
       </c>
       <c r="H60" s="32">
-        <f t="shared" si="5"/>
-        <v>203.74295040000001</v>
+        <f t="shared" si="4"/>
+        <v>204.22575360000002</v>
       </c>
       <c r="I60" s="13"/>
       <c r="J60" s="1">
-        <f t="shared" si="11"/>
-        <v>0.56595123333333774</v>
+        <f>$J$63*(E60/15)</f>
+        <v>0.56729235000000455</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="28">
-        <f t="shared" si="13"/>
-        <v>0.30000000000001137</v>
+        <f t="shared" si="10"/>
+        <v>9.9999999999994316E-2</v>
       </c>
       <c r="B61" s="22">
-        <v>126.9</v>
+        <v>127</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E61" s="24">
-        <f t="shared" si="10"/>
-        <v>204.225246</v>
+        <f t="shared" si="8"/>
+        <v>204.38618</v>
       </c>
       <c r="F61" s="30">
-        <f t="shared" si="12"/>
-        <v>0.48280200000002083</v>
+        <f t="shared" si="9"/>
+        <v>0.16093399999999747</v>
       </c>
       <c r="G61" s="31">
-        <f t="shared" si="4"/>
-        <v>0.48000000000001819</v>
+        <f t="shared" si="3"/>
+        <v>0.1599999999999909</v>
       </c>
       <c r="H61" s="32">
-        <f t="shared" si="5"/>
-        <v>204.22575360000002</v>
+        <f t="shared" si="4"/>
+        <v>204.38668800000002</v>
       </c>
       <c r="I61" s="13"/>
       <c r="J61" s="1">
-        <f t="shared" si="11"/>
-        <v>0.56729235000000455</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+        <f>$J$63*(E61/15)</f>
+        <v>0.56773938888889341</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A62" s="28">
-        <f t="shared" si="13"/>
-        <v>9.9999999999994316E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.29999999999999716</v>
       </c>
       <c r="B62" s="22">
-        <v>127</v>
+        <v>127.3</v>
       </c>
       <c r="C62" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D62" s="29" t="s">
-        <v>77</v>
+      <c r="D62" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="E62" s="24">
-        <f t="shared" si="10"/>
-        <v>204.38618</v>
+        <f t="shared" si="8"/>
+        <v>204.86898199999999</v>
       </c>
       <c r="F62" s="30">
-        <f t="shared" si="12"/>
-        <v>0.16093399999999747</v>
+        <f t="shared" si="9"/>
+        <v>0.4828019999999924</v>
       </c>
       <c r="G62" s="31">
-        <f t="shared" si="4"/>
-        <v>0.1599999999999909</v>
+        <f t="shared" si="3"/>
+        <v>0.47999999999999543</v>
       </c>
       <c r="H62" s="32">
-        <f t="shared" si="5"/>
-        <v>204.38668800000002</v>
+        <f t="shared" si="4"/>
+        <v>204.8694912</v>
       </c>
       <c r="I62" s="13"/>
       <c r="J62" s="1">
-        <f t="shared" si="11"/>
-        <v>0.56773938888889341</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="56" x14ac:dyDescent="0.15">
-      <c r="A63" s="28">
-        <f t="shared" si="13"/>
-        <v>9.9999999999994316E-2</v>
-      </c>
-      <c r="B63" s="22">
-        <v>127.1</v>
-      </c>
-      <c r="C63" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E63" s="24">
-        <f t="shared" si="10"/>
-        <v>204.54711399999999</v>
-      </c>
-      <c r="F63" s="30">
-        <f t="shared" si="12"/>
-        <v>0.16093399999999747</v>
-      </c>
-      <c r="G63" s="31">
-        <f t="shared" si="4"/>
-        <v>0.1599999999999909</v>
-      </c>
-      <c r="H63" s="32">
-        <f t="shared" si="5"/>
-        <v>204.54762239999999</v>
-      </c>
-      <c r="I63" s="13"/>
-      <c r="J63" s="1">
-        <f t="shared" si="11"/>
-        <v>0.56818642777778228</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="21"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="34"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="4">
+        <f>$J$63*(E62/15)</f>
+        <v>0.56908050555556</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="21"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="4">
         <v>4.1666666666666997E-2</v>
       </c>
     </row>
-    <row r="65" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B65" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
+    <row r="64" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B64" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B64:D64"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions gridLines="1"/>
-  <pageMargins left="0.35" right="0.35" top="1" bottom="0.25" header="0" footer="0"/>
+  <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;CAlsea Loop brevet from Eugene, OR _x000D_Permanent #1726, Modified August 2017</oddHeader>
+  </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="27" max="7" man="1"/>
   </rowBreaks>
@@ -3339,11 +3529,11 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>113.8</v>
+        <v>113.3</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>11.299999999999997</v>
+        <v>10.799999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -3351,11 +3541,11 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>127.1</v>
+        <v>127.3</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>13.299999999999997</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3368,4 +3558,970 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="6" width="10.83203125" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="39">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="39">
+        <v>479.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="39">
+        <v>5.74</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="39">
+        <v>446.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="39">
+        <v>9.01</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="39">
+        <v>498.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="39">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="39">
+        <v>408.14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="39">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="39">
+        <v>409.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="39">
+        <v>11.36</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="39">
+        <v>395.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="39">
+        <v>14.65</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="39">
+        <v>451.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="39">
+        <v>28.06</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="39">
+        <v>433.73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="39">
+        <v>30.66</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="39">
+        <v>328.74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="39">
+        <v>30.93</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="39">
+        <v>335.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="39">
+        <v>39.6</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="39">
+        <v>279.52999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="39">
+        <v>39.68</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="39">
+        <v>286.75</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="39">
+        <v>40.57</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="39">
+        <v>301.18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="39">
+        <v>41.43</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="39">
+        <v>294.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="39">
+        <v>42.28</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="39">
+        <v>290.35000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="39">
+        <v>44.25</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="39">
+        <v>347.77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="39">
+        <v>44.88</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="39">
+        <v>359.91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="39">
+        <v>45.53</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="39">
+        <v>333.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="39">
+        <v>53.08</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="39">
+        <v>257.87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="39">
+        <v>55.97</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="39">
+        <v>331.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="39">
+        <v>60.21</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="39">
+        <v>426.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="39">
+        <v>72.12</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="39">
+        <v>296.26</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="39">
+        <v>72.209999999999994</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="39">
+        <v>303.14999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="39">
+        <v>72.22</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="39">
+        <v>303.14999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="39">
+        <v>73.180000000000007</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="39">
+        <v>286.42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="39">
+        <v>86.1</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="39">
+        <v>1307.4100000000001</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="39">
+        <v>94.12</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="39">
+        <v>294.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="39">
+        <v>94.98</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="39">
+        <v>301.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="39">
+        <v>95.95</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="39">
+        <v>279.52999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="39">
+        <v>100.38</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="39">
+        <v>321.85000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="39">
+        <v>102.48</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="39">
+        <v>308.73</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="39">
+        <v>102.5</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="39">
+        <v>308.73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="39">
+        <v>105.05</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="39">
+        <v>312.66000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="39">
+        <v>105.55</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="39">
+        <v>324.14999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="39">
+        <v>107.09</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="39">
+        <v>332.68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="39">
+        <v>108.94</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" s="39">
+        <v>338.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="39">
+        <v>113.74</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" s="39">
+        <v>388.12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="39">
+        <v>114.24</v>
+      </c>
+      <c r="B40" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="39">
+        <v>374.34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="39">
+        <v>114.62</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="39">
+        <v>374.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="39">
+        <v>115.11</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" s="39">
+        <v>379.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="39">
+        <v>116.06</v>
+      </c>
+      <c r="B43" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43" s="39">
+        <v>388.45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="39">
+        <v>116.13</v>
+      </c>
+      <c r="B44" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="39">
+        <v>387.47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="39">
+        <v>116.3</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="39">
+        <v>383.53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="39">
+        <v>117.82</v>
+      </c>
+      <c r="B46" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" s="39">
+        <v>398.95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="39">
+        <v>119.12</v>
+      </c>
+      <c r="B47" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47" s="39">
+        <v>384.19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="39">
+        <v>119.14</v>
+      </c>
+      <c r="B48" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="39">
+        <v>384.19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="39">
+        <v>120.12</v>
+      </c>
+      <c r="B49" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="E49" s="39">
+        <v>384.19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="39">
+        <v>121.07</v>
+      </c>
+      <c r="B50" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" s="39">
+        <v>389.76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="39">
+        <v>121.11</v>
+      </c>
+      <c r="B51" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" s="39">
+        <v>389.11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="39">
+        <v>123.49</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="39">
+        <v>403.22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="39">
+        <v>123.68</v>
+      </c>
+      <c r="B53" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53" s="39">
+        <v>397.31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="39">
+        <v>124.3</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" s="39">
+        <v>400.59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="39">
+        <v>124.33</v>
+      </c>
+      <c r="B55" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="39">
+        <v>404.53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="39">
+        <v>124.91</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E56" s="39">
+        <v>403.87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" s="39">
+        <v>125.18</v>
+      </c>
+      <c r="B57" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57" s="39">
+        <v>408.79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" s="39">
+        <v>125.23</v>
+      </c>
+      <c r="B58" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="39">
+        <v>408.46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" s="39">
+        <v>125.24</v>
+      </c>
+      <c r="B59" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E59" s="39">
+        <v>406.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A60" s="39">
+        <v>125.4</v>
+      </c>
+      <c r="B60" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E60" s="39">
+        <v>407.48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A61" s="39">
+        <v>125.59</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="E61" s="39">
+        <v>422.24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A62" s="39">
+        <v>126.89</v>
+      </c>
+      <c r="B62" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="E62" s="39">
+        <v>595.79999999999995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A63" s="39">
+        <v>127.34</v>
+      </c>
+      <c r="B63" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="E63" s="39">
+        <v>479.66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A64" s="39">
+        <v>127.63</v>
+      </c>
+      <c r="B64" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E64" s="39">
+        <v>444.88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" s="39">
+        <v>127.87</v>
+      </c>
+      <c r="B65" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E65" s="39">
+        <v>461.29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;CRaw cues as exported from Ride with GPS_x000D_(columns rearranged)</oddHeader>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>